<commit_message>
improved mappings file: can provide OMIA id instead of phene id; phene name is put in NOTES field for annotations
</commit_message>
<xml_diff>
--- a/src/main/dist/data/RGD_OMIA_matching_20190911.xlsx
+++ b/src/main/dist/data/RGD_OMIA_matching_20190911.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="495">
   <si>
     <t>phene_name</t>
   </si>
@@ -1419,13 +1419,106 @@
   </si>
   <si>
     <t>DOID:308</t>
+  </si>
+  <si>
+    <t>VT:0010463</t>
+  </si>
+  <si>
+    <t>OMIA_ID</t>
+  </si>
+  <si>
+    <t>OMIM_NO</t>
+  </si>
+  <si>
+    <t>DOID:0111072</t>
+  </si>
+  <si>
+    <t>Leg weakness, MSTN-related</t>
+  </si>
+  <si>
+    <t>Mannosidosis, beta</t>
+  </si>
+  <si>
+    <t>DOID:3633</t>
+  </si>
+  <si>
+    <t>Hypophosphatasia</t>
+  </si>
+  <si>
+    <t>DOID:0110914</t>
+  </si>
+  <si>
+    <t>Diffuse cystic renal dysplasia and hepatic fibrosis</t>
+  </si>
+  <si>
+    <t>DOID:0110980</t>
+  </si>
+  <si>
+    <t>Congenital dyshormonogenic hypothyroidism with goiter</t>
+  </si>
+  <si>
+    <t>DOID:9008019</t>
+  </si>
+  <si>
+    <t>Amelogenesis imperfecta, ACP4-related</t>
+  </si>
+  <si>
+    <t>DOID:9002499</t>
+  </si>
+  <si>
+    <t>Stargardt disease 1</t>
+  </si>
+  <si>
+    <t>DOID:9006630</t>
+  </si>
+  <si>
+    <t>Cardiomyopathy, dilated, PLN-related</t>
+  </si>
+  <si>
+    <t>DOID:0110439</t>
+  </si>
+  <si>
+    <t>Deafness, unilateral and vestibular dysfunction</t>
+  </si>
+  <si>
+    <t>DOID:0110529</t>
+  </si>
+  <si>
+    <t>Coat colour, phaeomelanin dilution, MFSD12-related</t>
+  </si>
+  <si>
+    <t>Progressive retinal atrophy, NECAP1-related</t>
+  </si>
+  <si>
+    <t>Ehlers-Danlos syndrome, classic-like, 1</t>
+  </si>
+  <si>
+    <t>DOID:9003741</t>
+  </si>
+  <si>
+    <t>Ciliary dyskinesia, primary, NME5-related</t>
+  </si>
+  <si>
+    <t>DOID:9562</t>
+  </si>
+  <si>
+    <t>Bernard-Soulier syndrome, type C</t>
+  </si>
+  <si>
+    <t>DOID:9001316</t>
+  </si>
+  <si>
+    <t>Eye malformation, congenital</t>
+  </si>
+  <si>
+    <t>DOID:9002525</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1454,6 +1547,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1475,7 +1574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1494,6 +1593,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1816,10 +1919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D262"/>
+  <dimension ref="A1:F277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C251" sqref="C251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1827,9 +1931,10 @@
     <col min="2" max="2" width="59.25" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>205</v>
       </c>
@@ -1842,8 +1947,14 @@
       <c r="D1" s="3" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>16</v>
       </c>
@@ -1854,7 +1965,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>31</v>
       </c>
@@ -1865,7 +1976,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>50</v>
       </c>
@@ -1876,7 +1987,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>54</v>
       </c>
@@ -1887,7 +1998,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>56</v>
       </c>
@@ -1901,7 +2012,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>58</v>
       </c>
@@ -1915,7 +2026,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>101</v>
       </c>
@@ -1926,7 +2037,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>170</v>
       </c>
@@ -1937,7 +2048,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>316</v>
       </c>
@@ -1948,7 +2059,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>319</v>
       </c>
@@ -1962,7 +2073,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>372</v>
       </c>
@@ -1976,7 +2087,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>373</v>
       </c>
@@ -1990,16 +2101,21 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>435</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D14" s="10">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>443</v>
       </c>
@@ -2013,7 +2129,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>465</v>
       </c>
@@ -2704,14 +2820,19 @@
         <v>262</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>2159</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C75" s="7"/>
+      <c r="C75" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D75" s="10">
+        <v>43720</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
@@ -2967,14 +3088,19 @@
         <v>307</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>2695</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C98" s="7"/>
+      <c r="C98" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D98" s="10">
+        <v>43720</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
@@ -3111,14 +3237,19 @@
         <v>315</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
         <v>2788</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C111" s="7"/>
+      <c r="C111" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D111" s="10">
+        <v>43720</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="6">
@@ -3134,7 +3265,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
         <v>2822</v>
       </c>
@@ -3148,7 +3279,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>2845</v>
       </c>
@@ -3159,16 +3290,21 @@
         <v>320</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>2865</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C115" s="7"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C115" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D115" s="10">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>2866</v>
       </c>
@@ -3179,7 +3315,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="6">
         <v>2885</v>
       </c>
@@ -3189,8 +3325,14 @@
       <c r="C117" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D117" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E117">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="6">
         <v>2888</v>
       </c>
@@ -3201,7 +3343,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="6">
         <v>2890</v>
       </c>
@@ -3212,7 +3354,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>2900</v>
       </c>
@@ -3223,7 +3365,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="6">
         <v>2901</v>
       </c>
@@ -3234,7 +3376,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="6">
         <v>2904</v>
       </c>
@@ -3245,7 +3387,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="6">
         <v>2922</v>
       </c>
@@ -3256,7 +3398,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>2926</v>
       </c>
@@ -3267,7 +3409,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>2927</v>
       </c>
@@ -3281,7 +3423,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="6">
         <v>2957</v>
       </c>
@@ -3292,7 +3434,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="6">
         <v>2961</v>
       </c>
@@ -3303,7 +3445,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>2973</v>
       </c>
@@ -3490,7 +3632,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="6">
         <v>2998</v>
       </c>
@@ -3501,7 +3643,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="6">
         <v>2999</v>
       </c>
@@ -3512,7 +3654,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="6">
         <v>3008</v>
       </c>
@@ -3521,7 +3663,7 @@
       </c>
       <c r="C147" s="7"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="6">
         <v>3009</v>
       </c>
@@ -3532,16 +3674,21 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="6">
         <v>3027</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C149" s="7"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C149" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D149" s="10">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="6">
         <v>3042</v>
       </c>
@@ -3552,7 +3699,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="6">
         <v>3060</v>
       </c>
@@ -3563,7 +3710,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="6">
         <v>3062</v>
       </c>
@@ -3574,7 +3721,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="6">
         <v>3065</v>
       </c>
@@ -3585,7 +3732,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="6">
         <v>3066</v>
       </c>
@@ -3596,7 +3743,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="6">
         <v>3076</v>
       </c>
@@ -3607,7 +3754,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="6">
         <v>3079</v>
       </c>
@@ -3618,7 +3765,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="6">
         <v>3094</v>
       </c>
@@ -3629,7 +3776,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="6">
         <v>3095</v>
       </c>
@@ -3640,7 +3787,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A159" s="6">
         <v>3096</v>
       </c>
@@ -3651,7 +3798,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
         <v>3097</v>
       </c>
@@ -3706,14 +3853,19 @@
         <v>350</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="6">
         <v>3117</v>
       </c>
       <c r="B165" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C165" s="7"/>
+      <c r="C165" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D165" s="10">
+        <v>43720</v>
+      </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="6">
@@ -3991,14 +4143,19 @@
         <v>363</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
         <v>3513</v>
       </c>
       <c r="B190" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C190" s="7"/>
+      <c r="C190" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D190" s="10">
+        <v>43720</v>
+      </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="6">
@@ -4583,7 +4740,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" s="6">
         <v>4000</v>
       </c>
@@ -4597,7 +4754,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" s="6">
         <v>4005</v>
       </c>
@@ -4608,7 +4765,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" s="6">
         <v>4007</v>
       </c>
@@ -4622,7 +4779,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" s="6">
         <v>4009</v>
       </c>
@@ -4636,7 +4793,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" s="6">
         <v>4011</v>
       </c>
@@ -4647,7 +4804,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" s="7">
         <v>4026</v>
       </c>
@@ -4661,7 +4818,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" s="7">
         <v>4033</v>
       </c>
@@ -4675,7 +4832,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" s="7">
         <v>4037</v>
       </c>
@@ -4689,7 +4846,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" s="7">
         <v>4047</v>
       </c>
@@ -4703,7 +4860,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" s="7">
         <v>4052</v>
       </c>
@@ -4717,7 +4874,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" s="7">
         <v>4053</v>
       </c>
@@ -4728,10 +4885,16 @@
         <v>453</v>
       </c>
       <c r="D251" s="10">
-        <v>43502</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43720</v>
+      </c>
+      <c r="E251">
+        <v>2122</v>
+      </c>
+      <c r="F251">
+        <v>601287</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" s="7">
         <v>4063</v>
       </c>
@@ -4745,7 +4908,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" s="7">
         <v>4067</v>
       </c>
@@ -4759,7 +4922,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" s="7">
         <v>4072</v>
       </c>
@@ -4773,7 +4936,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" s="7">
         <v>4073</v>
       </c>
@@ -4787,7 +4950,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" s="7">
         <v>4083</v>
       </c>
@@ -4801,7 +4964,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" s="7">
         <v>4088</v>
       </c>
@@ -4815,7 +4978,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" s="7">
         <v>4089</v>
       </c>
@@ -4829,7 +4992,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
         <v>4098</v>
       </c>
@@ -4843,7 +5006,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" s="7">
         <v>4118</v>
       </c>
@@ -4857,7 +5020,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" s="7">
         <v>4119</v>
       </c>
@@ -4871,7 +5034,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" s="7">
         <v>4127</v>
       </c>
@@ -4883,6 +5046,255 @@
       </c>
       <c r="D262" s="10">
         <v>43502</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B263" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="C263" t="s">
+        <v>467</v>
+      </c>
+      <c r="D263" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E263">
+        <v>2161</v>
+      </c>
+      <c r="F263">
+        <v>614160</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B264" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="C264" t="s">
+        <v>470</v>
+      </c>
+      <c r="D264" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E264">
+        <v>626</v>
+      </c>
+      <c r="F264">
+        <v>248510</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B265" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="C265" t="s">
+        <v>472</v>
+      </c>
+      <c r="D265" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E265">
+        <v>2162</v>
+      </c>
+      <c r="F265">
+        <v>241500</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B266" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C266" t="s">
+        <v>474</v>
+      </c>
+      <c r="D266" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E266">
+        <v>2173</v>
+      </c>
+      <c r="F266">
+        <v>213300</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B267" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="C267" t="s">
+        <v>476</v>
+      </c>
+      <c r="D267" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E267">
+        <v>2174</v>
+      </c>
+      <c r="F267">
+        <v>274400</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B268" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="C268" t="s">
+        <v>478</v>
+      </c>
+      <c r="D268" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E268">
+        <v>2177</v>
+      </c>
+      <c r="F268">
+        <v>617297</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B269" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="C269" t="s">
+        <v>480</v>
+      </c>
+      <c r="D269" s="10">
+        <v>40068</v>
+      </c>
+      <c r="E269">
+        <v>2179</v>
+      </c>
+      <c r="F269">
+        <v>248200</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B270" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="C270" t="s">
+        <v>482</v>
+      </c>
+      <c r="D270" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E270">
+        <v>2195</v>
+      </c>
+      <c r="F270">
+        <v>609909</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B271" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="C271" t="s">
+        <v>484</v>
+      </c>
+      <c r="D271" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E271">
+        <v>2196</v>
+      </c>
+      <c r="F271">
+        <v>613391</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B272" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="C272" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D272" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E272">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="273" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B273" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="C273" t="s">
+        <v>300</v>
+      </c>
+      <c r="D273" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E273">
+        <v>2198</v>
+      </c>
+      <c r="F273">
+        <v>611623</v>
+      </c>
+    </row>
+    <row r="274" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B274" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="C274" t="s">
+        <v>488</v>
+      </c>
+      <c r="D274" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E274">
+        <v>2203</v>
+      </c>
+      <c r="F274">
+        <v>606408</v>
+      </c>
+    </row>
+    <row r="275" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B275" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="C275" t="s">
+        <v>490</v>
+      </c>
+      <c r="D275" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E275">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="276" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B276" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="C276" t="s">
+        <v>492</v>
+      </c>
+      <c r="D276" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E276">
+        <v>2207</v>
+      </c>
+      <c r="F276">
+        <v>231200</v>
+      </c>
+    </row>
+    <row r="277" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B277" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="C277" t="s">
+        <v>494</v>
+      </c>
+      <c r="D277" s="10">
+        <v>43720</v>
+      </c>
+      <c r="E277">
+        <v>2208</v>
+      </c>
+      <c r="F277">
+        <v>212550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>